<commit_message>
delete working of last week
</commit_message>
<xml_diff>
--- a/应用软件周报.xlsx
+++ b/应用软件周报.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="4"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="130">
   <si>
     <t>组别</t>
   </si>
@@ -581,7 +581,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -4390,7 +4390,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4425,7 +4425,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -10531,8 +10531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.15"/>
@@ -10632,9 +10632,7 @@
       <c r="E4" s="56" t="s">
         <v>95</v>
       </c>
-      <c r="F4" s="47" t="s">
-        <v>87</v>
-      </c>
+      <c r="F4" s="47"/>
       <c r="G4" s="47" t="s">
         <v>88</v>
       </c>

</xml_diff>